<commit_message>
se agrego carpeta del tercer parcial y se agrego el nuevo tema de listas
</commit_message>
<xml_diff>
--- a/SecondPartial/pruebas de escritorio.xlsx
+++ b/SecondPartial/pruebas de escritorio.xlsx
@@ -5,17 +5,19 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rodri\Desktop\EstructuraDeDatos\SecondPartial\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rodri\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DEBDE662-E1AF-4D4B-9209-1B1BCA941D9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F9BB88-4430-48A4-A1D4-8BA082A605B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="2" xr2:uid="{839960C1-F96B-4C15-A7DB-8EC0806AA2BF}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="3" xr2:uid="{839960C1-F96B-4C15-A7DB-8EC0806AA2BF}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
+    <sheet name="insercion" sheetId="1" r:id="rId1"/>
+    <sheet name="seleccion" sheetId="2" r:id="rId2"/>
+    <sheet name="bubble" sheetId="3" r:id="rId3"/>
+    <sheet name="merge" sheetId="4" r:id="rId4"/>
+    <sheet name="quick" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="128">
   <si>
     <t>Iteración</t>
   </si>
@@ -597,13 +599,177 @@
   </si>
   <si>
     <t>resultado</t>
+  </si>
+  <si>
+    <t>Paso</t>
+  </si>
+  <si>
+    <t>Subarreglo Original</t>
+  </si>
+  <si>
+    <t>Subarreglos a Dividir</t>
+  </si>
+  <si>
+    <t>Comparación</t>
+  </si>
+  <si>
+    <t>Elementos Comparados</t>
+  </si>
+  <si>
+    <t>Resultado de la Comparación</t>
+  </si>
+  <si>
+    <t>Subarreglo Resultante</t>
+  </si>
+  <si>
+    <t>{5, 2, 9, 1, 5}</t>
+  </si>
+  <si>
+    <t>{5, 2, 9} - {1, 5}</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>{5, 2, 9}</t>
+  </si>
+  <si>
+    <t>{5, 2} - {9}</t>
+  </si>
+  <si>
+    <t>5 y 2</t>
+  </si>
+  <si>
+    <t>5 &gt; 2</t>
+  </si>
+  <si>
+    <t>{2, 5}</t>
+  </si>
+  <si>
+    <t>{2, 5} - {9}</t>
+  </si>
+  <si>
+    <t>5 y 9</t>
+  </si>
+  <si>
+    <t>5 &lt; 9</t>
+  </si>
+  <si>
+    <t>{2, 5, 9}</t>
+  </si>
+  <si>
+    <t>{1, 5}</t>
+  </si>
+  <si>
+    <t>{1} - {5}</t>
+  </si>
+  <si>
+    <t>1 y 5</t>
+  </si>
+  <si>
+    <t>1 &lt; 5</t>
+  </si>
+  <si>
+    <t>{2, 5, 9} y {1, 5}</t>
+  </si>
+  <si>
+    <t>2 y 1</t>
+  </si>
+  <si>
+    <t>2 &gt; 1</t>
+  </si>
+  <si>
+    <t>{1}</t>
+  </si>
+  <si>
+    <t>5 y 1</t>
+  </si>
+  <si>
+    <t>5 &gt; 1</t>
+  </si>
+  <si>
+    <t>{1, 2}</t>
+  </si>
+  <si>
+    <t>5 y 5</t>
+  </si>
+  <si>
+    <t>5 = 5</t>
+  </si>
+  <si>
+    <t>{1, 2, 5}</t>
+  </si>
+  <si>
+    <t>9 y 5</t>
+  </si>
+  <si>
+    <t>9 &gt; 5</t>
+  </si>
+  <si>
+    <t>{1, 2, 5, 5}</t>
+  </si>
+  <si>
+    <t>{1, 2, 5, 5, 9}</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Llamada a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>quicksort</t>
+    </r>
+  </si>
+  <si>
+    <t>Subarreglo</t>
+  </si>
+  <si>
+    <t>Pivote</t>
+  </si>
+  <si>
+    <t>Intercambios</t>
+  </si>
+  <si>
+    <t>Resultado Parcial</t>
+  </si>
+  <si>
+    <t>quicksort(a, 0, 4)</t>
+  </si>
+  <si>
+    <t>[5, 2, 9, 1, 5]</t>
+  </si>
+  <si>
+    <t>[2, 1, 5, 5, 9]</t>
+  </si>
+  <si>
+    <t>quicksort(a, 0, 1)</t>
+  </si>
+  <si>
+    <t>[2, 1]</t>
+  </si>
+  <si>
+    <t>[1, 2, 5, 5, 9]</t>
+  </si>
+  <si>
+    <t>quicksort(a, 3, 4)</t>
+  </si>
+  <si>
+    <t>[5, 9]</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -629,6 +795,14 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -720,31 +894,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -763,6 +928,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1102,7 +1276,7 @@
   <dimension ref="B2:I12"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15:I17"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -1136,7 +1310,7 @@
       <c r="G2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="6" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1144,114 +1318,114 @@
       <c r="B3" s="1">
         <v>1</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="3">
         <v>1</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="3">
         <v>4</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8" t="s">
+      <c r="H3" s="5"/>
+      <c r="I3" s="5" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="22.15" customHeight="1">
-      <c r="B4" s="12">
+      <c r="B4" s="9">
         <v>2</v>
       </c>
-      <c r="C4" s="13">
+      <c r="C4" s="10">
         <v>2</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="10">
         <v>3</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="I4" s="7" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="19.899999999999999" customHeight="1">
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="7" t="s">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="2:9" ht="36.4" customHeight="1">
-      <c r="B6" s="15">
+      <c r="B6" s="12">
         <v>3</v>
       </c>
-      <c r="C6" s="16">
+      <c r="C6" s="13">
         <v>3</v>
       </c>
-      <c r="D6" s="16">
+      <c r="D6" s="13">
         <v>2</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="G6" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="I6" s="10" t="s">
+      <c r="I6" s="7" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="18.399999999999999" customHeight="1">
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="7" t="s">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="4" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="8" spans="2:9" ht="55.9" customHeight="1">
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="7" t="s">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="11" t="s">
+      <c r="I8" s="8" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1259,64 +1433,64 @@
       <c r="B9" s="1">
         <v>4</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="3">
         <v>4</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="3">
         <v>1</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="10" spans="2:9" ht="19.149999999999999" customHeight="1">
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="7" t="s">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G10" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="I10" s="10" t="s">
+      <c r="I10" s="7" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="11" spans="2:9" ht="18" customHeight="1">
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="7" t="s">
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G11" s="4" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="12" spans="2:9" ht="18" customHeight="1">
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="7" t="s">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="F12" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="G12" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1330,7 +1504,7 @@
   <dimension ref="B2:I7"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -1366,22 +1540,22 @@
       <c r="B3" s="1">
         <v>1</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="3">
         <v>0</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="7" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1389,19 +1563,19 @@
       <c r="B4" s="1">
         <v>2</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="3">
         <v>1</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1409,22 +1583,22 @@
       <c r="B5" s="1">
         <v>3</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="3">
         <v>2</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="I5" s="7" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1432,19 +1606,19 @@
       <c r="B6" s="1">
         <v>4</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="3">
         <v>3</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1452,22 +1626,22 @@
       <c r="B7" s="1">
         <v>5</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="3">
         <v>4</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="I7" s="7" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1480,8 +1654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C17418E1-6D07-45BE-9C03-3CBE9F683270}">
   <dimension ref="B2:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U11" sqref="U11"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -1503,13 +1677,13 @@
       </c>
     </row>
     <row r="3" spans="2:6">
-      <c r="B3" s="3">
+      <c r="B3" s="1">
         <v>1</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>66</v>
       </c>
       <c r="F3" t="s">
@@ -1517,35 +1691,35 @@
       </c>
     </row>
     <row r="4" spans="2:6">
-      <c r="B4" s="3">
+      <c r="B4" s="1">
         <v>2</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="5" spans="2:6">
-      <c r="B5" s="3">
+      <c r="B5" s="1">
         <v>3</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="6" spans="2:6">
-      <c r="B6" s="3">
+      <c r="B6" s="1">
         <v>4</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F6" t="s">
@@ -1553,19 +1727,414 @@
       </c>
     </row>
     <row r="7" spans="2:6">
-      <c r="B7" s="3">
+      <c r="B7" s="1">
         <v>5</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="2:6">
       <c r="F8" t="s">
         <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EDF2D6D-C231-407D-BBDF-A98318FFF22A}">
+  <dimension ref="B2:I11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <cols>
+    <col min="5" max="5" width="11.796875" customWidth="1"/>
+    <col min="6" max="6" width="12.59765625" customWidth="1"/>
+    <col min="7" max="7" width="11.86328125" customWidth="1"/>
+    <col min="9" max="9" width="15.73046875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9" ht="42.75">
+      <c r="B2" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="I2" s="16"/>
+    </row>
+    <row r="3" spans="2:9" ht="28.5">
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="I3" s="15"/>
+    </row>
+    <row r="4" spans="2:9">
+      <c r="B4" s="3">
+        <v>2</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="I4" s="15"/>
+    </row>
+    <row r="5" spans="2:9">
+      <c r="B5" s="3">
+        <v>3</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E5" s="3">
+        <v>2</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="I5" s="15"/>
+    </row>
+    <row r="6" spans="2:9">
+      <c r="B6" s="3">
+        <v>4</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E6" s="3">
+        <v>3</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="I6" s="15"/>
+    </row>
+    <row r="7" spans="2:9" ht="28.5">
+      <c r="B7" s="3">
+        <v>5</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E7" s="3">
+        <v>4</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="I7" s="15"/>
+    </row>
+    <row r="8" spans="2:9" ht="28.5">
+      <c r="B8" s="3">
+        <v>6</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E8" s="3">
+        <v>5</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="I8" s="15"/>
+    </row>
+    <row r="9" spans="2:9" ht="28.5">
+      <c r="B9" s="3">
+        <v>7</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E9" s="3">
+        <v>6</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="I9" s="15"/>
+    </row>
+    <row r="10" spans="2:9" ht="28.5">
+      <c r="B10" s="3">
+        <v>8</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E10" s="3">
+        <v>7</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="I10" s="15"/>
+    </row>
+    <row r="11" spans="2:9" ht="28.5">
+      <c r="B11" s="3">
+        <v>9</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E11" s="3">
+        <v>8</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="I11" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1135EF23-B069-4DCB-844A-F3E7497B476F}">
+  <dimension ref="B2:H6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <cols>
+    <col min="4" max="4" width="11.3984375" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" ht="28.5">
+      <c r="B2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" ht="25.5">
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="E3" s="4">
+        <v>5</v>
+      </c>
+      <c r="F3" s="4">
+        <v>4</v>
+      </c>
+      <c r="G3" s="4">
+        <v>4</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="25.5">
+      <c r="B4" s="3">
+        <v>2</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="4">
+        <v>1</v>
+      </c>
+      <c r="G4" s="4">
+        <v>1</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="25.5">
+      <c r="B5" s="3">
+        <v>3</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="E5" s="4">
+        <v>9</v>
+      </c>
+      <c r="F5" s="4">
+        <v>1</v>
+      </c>
+      <c r="G5" s="4">
+        <v>1</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="25.5">
+      <c r="B6" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F6" s="1">
+        <v>7</v>
+      </c>
+      <c r="G6" s="1">
+        <v>7</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>